<commit_message>
completed the mini project number 1
</commit_message>
<xml_diff>
--- a/01_LinuxLearning/00_Projects/01_MiniProject_ChatApplication/01_Design/ApplicationSpecification.xlsx
+++ b/01_LinuxLearning/00_Projects/01_MiniProject_ChatApplication/01_Design/ApplicationSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_GitProject\99_Learning\01_LinuxLearning\00_Projects\01_MiniProject_ChatApplication\01_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54055BA4-7F7D-465B-BFAC-EFDAFDE4E9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F8425A-C88A-42F6-AFA3-958394EF39AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -207,9 +206,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Not implemented</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -622,6 +618,9 @@
   </si>
   <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>Released</t>
   </si>
 </sst>
 </file>
@@ -1043,13 +1042,13 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1057,7 +1056,7 @@
     <col min="4" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="118.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -1099,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>2</v>
@@ -1123,7 +1122,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>9</v>
@@ -1147,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>3</v>
@@ -1171,10 +1170,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1193,10 +1192,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1215,10 +1214,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -1237,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
@@ -1261,10 +1260,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -1283,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>10</v>
@@ -1307,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>11</v>
@@ -1329,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>12</v>
@@ -1351,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>13</v>
@@ -1373,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>5</v>
@@ -1397,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -1419,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>6</v>
@@ -1443,10 +1442,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -1465,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>14</v>
@@ -1487,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>7</v>
@@ -1511,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1533,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>15</v>
@@ -1555,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>16</v>
@@ -1579,7 +1578,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>17</v>
@@ -1601,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>18</v>
@@ -1623,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>19</v>
@@ -1645,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>8</v>
@@ -1669,10 +1668,10 @@
         <v>2</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -1691,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>20</v>
@@ -1713,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>22</v>
@@ -1737,7 +1736,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>42</v>
@@ -1759,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>43</v>
@@ -1781,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>23</v>
@@ -1805,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>44</v>
@@ -1827,7 +1826,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>45</v>
@@ -1849,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>24</v>
@@ -1873,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>37</v>
@@ -1897,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>39</v>
@@ -1919,7 +1918,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>40</v>
@@ -1941,7 +1940,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>41</v>
@@ -1963,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>38</v>
@@ -1985,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>25</v>
@@ -2009,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>35</v>
@@ -2031,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>36</v>
@@ -2053,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>26</v>
@@ -2077,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>32</v>
@@ -2099,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>33</v>
@@ -2121,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>34</v>
@@ -2143,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>27</v>
@@ -2167,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>28</v>
@@ -2189,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>29</v>
@@ -2211,7 +2210,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>30</v>
@@ -2233,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>31</v>
@@ -2253,7 +2252,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>